<commit_message>
updated parts and schematic
</commit_message>
<xml_diff>
--- a/Documentation/parts.xlsx
+++ b/Documentation/parts.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23CC028A-430A-425D-91FC-3203B7EE0EB0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD8C0D5-4A1C-4CF1-8A07-5673117AE22D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Amount</t>
   </si>
@@ -73,13 +73,10 @@
     <t>Light</t>
   </si>
   <si>
-    <t>Price2</t>
-  </si>
-  <si>
-    <t>Our Price</t>
-  </si>
-  <si>
     <t>Servomotor</t>
+  </si>
+  <si>
+    <t>Connector Strip</t>
   </si>
 </sst>
 </file>
@@ -177,13 +174,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     </dxf>
@@ -207,23 +198,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4677A303-366F-4D24-8031-5F3EC170E8BA}" name="Tabelle1" displayName="Tabelle1" ref="B4:F18" totalsRowCount="1">
-  <autoFilter ref="B4:F17" xr:uid="{E25B9ECC-1BED-4A59-BA65-37CFBAF8D359}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4677A303-366F-4D24-8031-5F3EC170E8BA}" name="Tabelle1" displayName="Tabelle1" ref="B4:E19" totalsRowCount="1">
+  <autoFilter ref="B4:E18" xr:uid="{E25B9ECC-1BED-4A59-BA65-37CFBAF8D359}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A05BF368-D9FD-4999-8EA6-0D0E96AACDA5}" name="Component" totalsRowLabel="Sum"/>
     <tableColumn id="2" xr3:uid="{82282FCE-F81E-4720-8752-2AA356D2D89F}" name="Amount"/>
-    <tableColumn id="3" xr3:uid="{552DE5D0-3C8B-4C7E-AF6F-C47A4CB978BF}" name="Price per piece" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{4797D94F-5034-4CBD-8FA3-6A194AAB3BD4}" name="Price" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="1">
+    <tableColumn id="3" xr3:uid="{552DE5D0-3C8B-4C7E-AF6F-C47A4CB978BF}" name="Price per piece" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4797D94F-5034-4CBD-8FA3-6A194AAB3BD4}" name="Price" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>C5*D5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{70B18C34-AF70-4080-82FC-6B2551C10EE1}" name="Price2" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
-      <calculatedColumnFormula>D5*E5</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Tabelle1[Price2])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -493,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F18"/>
+  <dimension ref="B4:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,12 +493,7 @@
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -524,29 +506,23 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <v>2.3980000000000001</v>
       </c>
       <c r="E5" s="2">
         <f>C5*D5</f>
-        <v>11.99</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -560,13 +536,10 @@
         <f t="shared" ref="E6:E7" si="0">C6*D6</f>
         <v>6.79</v>
       </c>
-      <c r="F6" s="2">
-        <v>6.79</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -578,11 +551,8 @@
         <f t="shared" si="0"/>
         <v>19.29</v>
       </c>
-      <c r="F7" s="2">
-        <v>19.29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -596,29 +566,23 @@
         <f t="shared" ref="E8:E14" si="1">C8*D8</f>
         <v>2.8899999999999997</v>
       </c>
-      <c r="F8" s="2">
-        <v>2.89</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2">
         <v>37.99</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
-        <v>37.99</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -626,35 +590,29 @@
         <v>1</v>
       </c>
       <c r="D10" s="8">
-        <v>0</v>
+        <v>8.3800000000000008</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <f>C10*D10</f>
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="9">
         <v>6</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
@@ -668,34 +626,28 @@
         <f t="shared" si="1"/>
         <v>3.35</v>
       </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="9">
         <v>0.17599999999999999</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="1"/>
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -704,11 +656,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -719,60 +668,62 @@
         <v>8.99</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" ref="E15:E17" si="2">C15*D15</f>
+        <f t="shared" ref="E15:E18" si="2">C15*D15</f>
         <v>8.99</v>
       </c>
-      <c r="F15" s="2">
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9">
+        <v>8.49</v>
+      </c>
+      <c r="E16" s="2">
+        <f>C16*D16</f>
+        <v>8.49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9">
         <v>9.99</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="2">
         <f t="shared" si="2"/>
         <v>9.99</v>
       </c>
-      <c r="F16" s="2">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9">
         <v>7.99</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E18" s="2">
         <f t="shared" si="2"/>
         <v>7.99</v>
       </c>
-      <c r="F17" s="2">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="2">
         <f>SUBTOTAL(109,Tabelle1[Price])</f>
-        <v>115.44599999999998</v>
-      </c>
-      <c r="F18" s="2">
-        <f>SUM(Tabelle1[Price2])</f>
-        <v>55.940000000000005</v>
+        <v>76.16</v>
       </c>
     </row>
   </sheetData>
@@ -785,14 +736,16 @@
     <hyperlink ref="B13" r:id="rId6" xr:uid="{9D9BDE6E-7BEE-4DAE-82AB-02EE2D977D81}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{50137844-70CA-40A5-965E-E5AB4DA72B33}"/>
     <hyperlink ref="B15" r:id="rId8" display="Power Supply Water pump" xr:uid="{1001E750-7B62-472D-81DA-A6F77D443A5A}"/>
-    <hyperlink ref="B16" r:id="rId9" xr:uid="{C6A98FEC-5564-4B36-90A6-793DC19E4E9D}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{C6A98FEC-5564-4B36-90A6-793DC19E4E9D}"/>
     <hyperlink ref="B7" r:id="rId10" xr:uid="{241E2F4A-EFB4-443A-B52E-BB27B6DB303F}"/>
-    <hyperlink ref="B17" r:id="rId11" xr:uid="{A8C1DFF2-5535-44BA-A132-14CF8FA21F0F}"/>
+    <hyperlink ref="B18" r:id="rId11" xr:uid="{A8C1DFF2-5535-44BA-A132-14CF8FA21F0F}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{C0F45065-666F-4AE5-B70E-A10C7E959743}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{CF79B9CC-0F4C-4766-BB70-5EC8EDC0B51F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ghpi library update, new pcb schematic
</commit_message>
<xml_diff>
--- a/Documentation/parts.xlsx
+++ b/Documentation/parts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD8C0D5-4A1C-4CF1-8A07-5673117AE22D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2844B0E0-8129-4E74-99F3-3F20A9BB45E8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Amount</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>DRV8825 Stepper Motor Driver</t>
-  </si>
-  <si>
     <t>DHT22 Temperature and Humidity Sensor</t>
   </si>
   <si>
@@ -77,16 +74,23 @@
   </si>
   <si>
     <t>Connector Strip</t>
+  </si>
+  <si>
+    <t>Other stuff</t>
+  </si>
+  <si>
+    <t>Price per Person</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +108,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,11 +168,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -169,6 +178,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -480,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:E19"/>
+  <dimension ref="B4:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,257 +509,265 @@
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2.3980000000000001</v>
-      </c>
-      <c r="E5" s="2">
-        <f>C5*D5</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6.79</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E6" si="0">C5*D5</f>
+        <v>6.79</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>6.79</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" ref="E6:E7" si="0">C6*D6</f>
-        <v>6.79</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="D6" s="1">
         <v>19.29</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>19.29</v>
       </c>
     </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7:E13" si="1">C7*D7</f>
+        <v>2.8899999999999997</v>
+      </c>
+    </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>37.99</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" ref="E8:E14" si="1">C8*D8</f>
-        <v>2.8899999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="E9" s="1">
+        <f>C9*D9</f>
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>37.99</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8">
-        <v>8.3800000000000008</v>
-      </c>
-      <c r="E10" s="2">
-        <f>C10*D10</f>
-        <v>8.3800000000000008</v>
-      </c>
-    </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7">
-        <v>0</v>
-      </c>
-      <c r="D11" s="9">
-        <v>6</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3.35</v>
+      </c>
+      <c r="E11" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9">
-        <v>3.35</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>3.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="7">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="7">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8">
+        <v>8.99</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" ref="E14:E17" si="2">C14*D14</f>
+        <v>8.99</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9">
-        <v>8.99</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" ref="E15:E18" si="2">C15*D15</f>
-        <v>8.99</v>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <v>8.49</v>
+      </c>
+      <c r="E15" s="1">
+        <f>C15*D15</f>
+        <v>8.49</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9">
-        <v>8.49</v>
-      </c>
-      <c r="E16" s="2">
-        <f>C16*D16</f>
-        <v>8.49</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8">
         <v>9.99</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E16" s="1">
         <f t="shared" si="2"/>
         <v>9.99</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8">
         <v>7.99</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E17" s="1">
         <f t="shared" si="2"/>
         <v>7.99</v>
       </c>
     </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1">
+        <f>C18*D18</f>
+        <v>25</v>
+      </c>
+    </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="2">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1">
         <f>SUBTOTAL(109,Tabelle1[Price])</f>
-        <v>76.16</v>
+        <v>97.81</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="13">
+        <f>Tabelle1[[#Totals],[Price]] / 4</f>
+        <v>24.452500000000001</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{AB6CFEFB-6B97-4570-9E31-3712803576B8}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{E9891F47-7580-493B-ADC7-768AE1E5B244}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{48380E5D-F4D8-492C-9DB5-179A34689800}"/>
-    <hyperlink ref="B11" r:id="rId4" xr:uid="{C4B67B45-B4D5-494E-89A6-1585ECA991D2}"/>
-    <hyperlink ref="B12" r:id="rId5" xr:uid="{854F0B3B-EF6E-4857-B6FD-809E9B03C700}"/>
-    <hyperlink ref="B13" r:id="rId6" xr:uid="{9D9BDE6E-7BEE-4DAE-82AB-02EE2D977D81}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{50137844-70CA-40A5-965E-E5AB4DA72B33}"/>
-    <hyperlink ref="B15" r:id="rId8" display="Power Supply Water pump" xr:uid="{1001E750-7B62-472D-81DA-A6F77D443A5A}"/>
-    <hyperlink ref="B17" r:id="rId9" xr:uid="{C6A98FEC-5564-4B36-90A6-793DC19E4E9D}"/>
-    <hyperlink ref="B7" r:id="rId10" xr:uid="{241E2F4A-EFB4-443A-B52E-BB27B6DB303F}"/>
-    <hyperlink ref="B18" r:id="rId11" xr:uid="{A8C1DFF2-5535-44BA-A132-14CF8FA21F0F}"/>
-    <hyperlink ref="B16" r:id="rId12" xr:uid="{C0F45065-666F-4AE5-B70E-A10C7E959743}"/>
-    <hyperlink ref="B10" r:id="rId13" xr:uid="{CF79B9CC-0F4C-4766-BB70-5EC8EDC0B51F}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{E9891F47-7580-493B-ADC7-768AE1E5B244}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{48380E5D-F4D8-492C-9DB5-179A34689800}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{854F0B3B-EF6E-4857-B6FD-809E9B03C700}"/>
+    <hyperlink ref="B12" r:id="rId4" xr:uid="{9D9BDE6E-7BEE-4DAE-82AB-02EE2D977D81}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{50137844-70CA-40A5-965E-E5AB4DA72B33}"/>
+    <hyperlink ref="B14" r:id="rId6" display="Power Supply Water pump" xr:uid="{1001E750-7B62-472D-81DA-A6F77D443A5A}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{C6A98FEC-5564-4B36-90A6-793DC19E4E9D}"/>
+    <hyperlink ref="B6" r:id="rId8" xr:uid="{241E2F4A-EFB4-443A-B52E-BB27B6DB303F}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{A8C1DFF2-5535-44BA-A132-14CF8FA21F0F}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{C0F45065-666F-4AE5-B70E-A10C7E959743}"/>
+    <hyperlink ref="B9" r:id="rId11" xr:uid="{CF79B9CC-0F4C-4766-BB70-5EC8EDC0B51F}"/>
+    <hyperlink ref="B10" r:id="rId12" xr:uid="{C4B67B45-B4D5-494E-89A6-1585ECA991D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>